<commit_message>
ajustes dos tipos de estudos
</commit_message>
<xml_diff>
--- a/SLR-ExtracaoDados.xlsx
+++ b/SLR-ExtracaoDados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="17900"/>
+    <workbookView xWindow="5560" yWindow="-14980" windowWidth="25600" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="2" r:id="rId1"/>
@@ -578,7 +578,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="461">
   <si>
     <t>Name</t>
   </si>
@@ -2190,6 +2190,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Euromicro Conference, 2001. Proceedings. 27th , vol., no., pp.233-239, 2001</t>
+  </si>
+  <si>
+    <t>"concentrates on practical questions and challenges facing the small companies." (p2 e p4)</t>
+  </si>
+  <si>
+    <t>XP+FDD+SCRUM</t>
+  </si>
+  <si>
+    <t>"the purpose of this paper is centred in suggesting a framework where we could obtain mutual benefits for using together maturity models and agile methods, taking advantage of the strengths of both contexts to apply them in COTS selection process specifying what we can do (with CMM) and how we can do it (with the best practices of agile methods) to obtain a successful COTS selection, and so providing coverage over main lessons learned reported from COTS projects. (p2)"</t>
+  </si>
+  <si>
+    <t>"These agile values can influence positively the COTS selection processes, and they can provide foundation to suggest agile practices to improve the agility in the COTS selection process.(p3)"</t>
+  </si>
+  <si>
+    <t>"On the other hand, in COTS discipline there are some important aspects that could be supported by agile methods, among others: the need for flexibility in user requirements definition [2, 4, 5, 8]; sharing knowledge between different kinds of disciplines that must work together in selection [3 - 6]; considering that human factors in COTS selection processes can help to improve project management, collaboration between stakeholders, and technical excellence [27, 11]. (p06)"</t>
   </si>
 </sst>
 </file>
@@ -3552,11 +3567,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="AE16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4783,13 +4798,13 @@
         <v>254</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>77</v>
+        <v>458</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>78</v>
+        <v>456</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>54</v>
+        <v>344</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>53</v>
@@ -4832,7 +4847,7 @@
       </c>
       <c r="Y14" s="14"/>
       <c r="Z14" s="14" t="s">
-        <v>84</v>
+        <v>457</v>
       </c>
       <c r="AA14" s="14" t="s">
         <v>85</v>
@@ -4854,13 +4869,13 @@
         <v>63</v>
       </c>
       <c r="AH14" s="14" t="s">
-        <v>86</v>
+        <v>459</v>
       </c>
       <c r="AI14" s="14" t="s">
         <v>87</v>
       </c>
       <c r="AJ14" s="15" t="s">
-        <v>82</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="75">
@@ -7037,7 +7052,7 @@
       </c>
     </row>
     <row r="38" spans="1:36" ht="45">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="54" t="s">
         <v>126</v>
       </c>
       <c r="B38" s="53">
@@ -7109,7 +7124,7 @@
       </c>
     </row>
     <row r="39" spans="1:36" ht="60">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="54" t="s">
         <v>127</v>
       </c>
       <c r="B39" s="53">
@@ -7911,7 +7926,7 @@
       </c>
     </row>
     <row r="47" spans="1:36" ht="30">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="54" t="s">
         <v>135</v>
       </c>
       <c r="B47" s="53">
@@ -8162,7 +8177,7 @@
       </c>
     </row>
     <row r="50" spans="1:36" ht="31" customHeight="1">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="54" t="s">
         <v>272</v>
       </c>
       <c r="B50" s="53">
@@ -8255,7 +8270,7 @@
       </c>
     </row>
     <row r="51" spans="1:36" ht="90">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="54" t="s">
         <v>273</v>
       </c>
       <c r="B51" s="53">
@@ -8751,7 +8766,7 @@
     <row r="58" spans="1:36">
       <c r="H58" s="58">
         <f ca="1">TODAY()</f>
-        <v>42452</v>
+        <v>42458</v>
       </c>
     </row>
     <row r="59" spans="1:36">
@@ -8762,11 +8777,11 @@
     <row r="60" spans="1:36">
       <c r="H60">
         <f ca="1">H59-H58</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I60" s="18">
         <f ca="1">H60*8</f>
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -8821,10 +8836,15 @@
     <hyperlink ref="A54" r:id="rId45"/>
     <hyperlink ref="A55" r:id="rId46"/>
     <hyperlink ref="A5" r:id="rId47"/>
+    <hyperlink ref="A50" r:id="rId48"/>
+    <hyperlink ref="A51" r:id="rId49"/>
+    <hyperlink ref="A47" r:id="rId50"/>
+    <hyperlink ref="A39" r:id="rId51"/>
+    <hyperlink ref="A38" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="26" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
-  <legacyDrawing r:id="rId48"/>
+  <legacyDrawing r:id="rId53"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ajustes na extracao para validacao do orientador
</commit_message>
<xml_diff>
--- a/SLR-ExtracaoDados.xlsx
+++ b/SLR-ExtracaoDados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="-14980" windowWidth="25600" windowHeight="14320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="2" r:id="rId1"/>
@@ -578,7 +578,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="486">
   <si>
     <t>Name</t>
   </si>
@@ -2195,9 +2195,6 @@
     <t>"concentrates on practical questions and challenges facing the small companies." (p2 e p4)</t>
   </si>
   <si>
-    <t>XP+FDD+SCRUM</t>
-  </si>
-  <si>
     <t>"the purpose of this paper is centred in suggesting a framework where we could obtain mutual benefits for using together maturity models and agile methods, taking advantage of the strengths of both contexts to apply them in COTS selection process specifying what we can do (with CMM) and how we can do it (with the best practices of agile methods) to obtain a successful COTS selection, and so providing coverage over main lessons learned reported from COTS projects. (p2)"</t>
   </si>
   <si>
@@ -2205,6 +2202,130 @@
   </si>
   <si>
     <t>"On the other hand, in COTS discipline there are some important aspects that could be supported by agile methods, among others: the need for flexibility in user requirements definition [2, 4, 5, 8]; sharing knowledge between different kinds of disciplines that must work together in selection [3 - 6]; considering that human factors in COTS selection processes can help to improve project management, collaboration between stakeholders, and technical excellence [27, 11]. (p06)"</t>
+  </si>
+  <si>
+    <t>"Metaphor (XP);
+Product Backlog (SCRUM); 
+Domain Object Modeling (FDD); 
+Planning game (XP);
+Pre-game planning and staging (SCRUM); 
+Staging (Crystal); 
+Small releases (XP)
+Pair Programming (XP);
+Collective Ownership (XP);
+Monitoring (SCRUM);
+Revision and Control (Crystal);
+Inspections (FDD) 
+Sprint Review Meeting (SCRUM);
+Feature teams (FDD); 
+Planning game (XP)
+Effort estimation (SCRUM); 
+Developing by feature (FDD);
+Testing (XP)
+On-site Customer (XP)
+Methodology tuning technique (Crystal);
+ Progress reporting (FDD)" (p08)</t>
+  </si>
+  <si>
+    <t>REQM; PP; PMC; SAM; MA; PPQA (p8)</t>
+  </si>
+  <si>
+    <t>XP+FDD+SCRUM+Crystal</t>
+  </si>
+  <si>
+    <t>"This study analyzes the influence of agile and CMMI contexts over COTS selection processes, which have generated controversy inside the software engineering community, with the purpose of suggesting an agreement point of reconciliation and balance among the necessary discipline required to develop a selection process, and the agility that we are able to provide to develop a COTS project. For this reason, we seek to take advantage of the discipline proposed in CMMI, and the agility of the best agile practices, to identify a point of balance that define the number of people involved in the COTS selection process development and the system criticality that should be having into account at the moment to carry out a COTS project. (p10)"</t>
+  </si>
+  <si>
+    <t>"[...] −There is a need for flexibility in defining requirements, because requirements
+engineering and COTS selection must be performed together [2 - 6].
+− In selection processes, it is necessary to involve the system users and to
+work together with them to understand and comprehend their real needs [3 - 7].
+− There is often little time available for COTS software selection, because it
+is required to operate in a commercial manner and a change in policy or in
+business processes may be requested at any time [3, 8].
+− Understanding the marketplace is vital in COTS selection, because there is a
+need for continuous technology watch to keep up with vendors [2, 3, 9].
+− Better techniques are needed for recording and managing information during
+COTS selection processes [5, 6, 7, 9]. (p1)"</t>
+  </si>
+  <si>
+    <t>Ethnografy</t>
+  </si>
+  <si>
+    <t>CMMi Level 1 ad-hoc</t>
+  </si>
+  <si>
+    <t>REQM; PP; PMC; SQA;</t>
+  </si>
+  <si>
+    <t>"[...] One thing to be stressed is that the conclusion derived may only be specialized to the studied organization. To apply the conclusion to other organizations, a further study must be conducted. Thus, ethnography and ethnographic analysis sometimes can be a previous study followed by other studies. (p853)"</t>
+  </si>
+  <si>
+    <t>"based on the agile manifesto in [1], a process model belongs to agile development methods may fit with the process inside the studied organization. (p853)"</t>
+  </si>
+  <si>
+    <t>" To move to maturity level 2, the organization must apply five CMM KPAs. The definition of each KPA is somehow too complex to be interpreted by the members of My-Software organization. (p854)"</t>
+  </si>
+  <si>
+    <t>"1. User stories
+2. On-site customer
+3. Release planning 
+4. Small releases
+5. Iteration planning
+6. Collective ownership 
+7. Continuous integration 
+8. Pair programming (p853, 854 and 855)"</t>
+  </si>
+  <si>
+    <t>"[...] In this research, how the process model applied in small scale software organization is studied. Then, a proposed SPI model is introduced and the application of the model is tailored to the specific context, thus, will derive benefits to the small software organization. (p852)"</t>
+  </si>
+  <si>
+    <t>interviews, memos, documentations from the organization, and many records of meetings</t>
+  </si>
+  <si>
+    <t>8 developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three years of business experience </t>
+  </si>
+  <si>
+    <t>"[...]to meet this KPA, we need additional mechanism outside the key practices of XP process model because there are no explicit core practices of XP that match with this KPA. (p855)"
+"[...] As a result of the study, a recommendation is proposed to help the small software organization. (p853)"</t>
+  </si>
+  <si>
+    <t>small scale software organizations</t>
+  </si>
+  <si>
+    <t>"(...) This paper provides an analysis of the effect of introducing Agile practices into a CMMI Level 5 company. (p1)"</t>
+  </si>
+  <si>
+    <t>Lean Software Dev + Scrum</t>
+  </si>
+  <si>
+    <t>"Lean has demonstrated notable results for many years in domains such as auto manufacturing, and has been adapted to other domains, including product and software development. (p5)"</t>
+  </si>
+  <si>
+    <t>Fundamental problems inherent in software development influenced the introduction of Scrum:
+* Uncertainty is inherent and inevitable in software development processes and products - 
+Ziv’s Uncertainty Principle [7]
+* For a new software system the requirements will not be completely known until after the 
+users have used it - Humphrey’s Requirements Uncertainty Principle [8] • It is not 
+possible to completely specify an interactive system – Wegner’s Lemma [9]
+* Ambiguous and changing requirements, combined with evolving tools and technologies make 
+implementation strategies unpredictable.</t>
+  </si>
+  <si>
+    <t>CMMi Level 3 and 4</t>
+  </si>
+  <si>
+    <t>"We believe that bad implementations are one of the main reasons for the existence of many negative criticisms of CMM. Such implementations are often characterized as in the table below, whereas many good CMM implementations address most of the criticism. (p4)"</t>
+  </si>
+  <si>
+    <t>healthcare business (p4)</t>
+  </si>
+  <si>
+    <t>"For Agile companies the article has presented how Generic Practices can be used to institutionalize agile practices and we presented Lean Software Development [19] as an operational tool to identify improvement opportunities in a CMMI 5 company. (p8)"
+"Our recommendation to the Agile community is to use the CMMI generic practices from CMMI Level 3 to amplify the benefits from Agile methods. Our recommendation to the CMMI community is to fit Agile methods into your CMMI framework. (p9)"</t>
   </si>
 </sst>
 </file>
@@ -2215,7 +2336,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2327,6 +2448,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2402,7 +2529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2425,8 +2552,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="339">
+  <cellStyleXfs count="343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2766,8 +2904,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2922,6 +3064,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="316" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="315" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2932,7 +3080,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="339">
+  <cellStyles count="343">
     <cellStyle name="Comma" xfId="315" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -3147,6 +3295,10 @@
     <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -3567,11 +3719,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="AE16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="AD16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ14" sqref="AJ14"/>
+      <selection pane="bottomRight" activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3597,9 +3749,11 @@
     <col min="19" max="22" width="11.33203125" customWidth="1"/>
     <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.33203125" customWidth="1"/>
-    <col min="25" max="25" width="19.1640625" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="14.83203125" customWidth="1"/>
-    <col min="27" max="29" width="13.33203125" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" customWidth="1"/>
     <col min="30" max="30" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.6640625" customWidth="1"/>
@@ -3611,14 +3765,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="28">
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
       <c r="K1" s="22" t="s">
         <v>36</v>
       </c>
@@ -4798,7 +4952,7 @@
         <v>254</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J14" s="15" t="s">
         <v>456</v>
@@ -4847,20 +5001,20 @@
       </c>
       <c r="Y14" s="14"/>
       <c r="Z14" s="14" t="s">
-        <v>457</v>
-      </c>
-      <c r="AA14" s="14" t="s">
-        <v>85</v>
+        <v>462</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>460</v>
       </c>
       <c r="AB14" s="14"/>
       <c r="AC14" s="14" t="s">
         <v>59</v>
       </c>
       <c r="AD14" s="14" t="s">
-        <v>83</v>
+        <v>461</v>
       </c>
       <c r="AE14" s="14" t="s">
-        <v>92</v>
+        <v>463</v>
       </c>
       <c r="AF14" s="14" t="s">
         <v>55</v>
@@ -4869,16 +5023,16 @@
         <v>63</v>
       </c>
       <c r="AH14" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="AI14" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="AJ14" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="AI14" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ14" s="15" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" ht="75">
+    </row>
+    <row r="15" spans="1:37" ht="45">
       <c r="A15" s="54" t="s">
         <v>103</v>
       </c>
@@ -4886,7 +5040,7 @@
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="63" t="s">
         <v>228</v>
       </c>
       <c r="D15" s="45" t="s">
@@ -4904,8 +5058,8 @@
       <c r="H15" s="45" t="s">
         <v>285</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>312</v>
+      <c r="I15" s="62" t="s">
+        <v>472</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>53</v>
@@ -4914,10 +5068,10 @@
         <v>54</v>
       </c>
       <c r="L15" s="55" t="s">
-        <v>313</v>
-      </c>
-      <c r="M15" t="s">
-        <v>65</v>
+        <v>465</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="N15" s="55" t="s">
         <v>55</v>
@@ -4925,59 +5079,56 @@
       <c r="O15" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="P15" s="55" t="s">
-        <v>314</v>
+      <c r="P15" s="56" t="s">
+        <v>473</v>
       </c>
       <c r="Q15" s="55" t="s">
         <v>90</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>316</v>
-      </c>
-      <c r="S15" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="T15" s="55" t="s">
-        <v>315</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
       <c r="U15" s="55" t="s">
-        <v>317</v>
+        <v>475</v>
       </c>
       <c r="V15" s="55" t="s">
-        <v>318</v>
-      </c>
-      <c r="W15" s="56" t="s">
-        <v>319</v>
+        <v>370</v>
+      </c>
+      <c r="W15" s="55" t="s">
+        <v>477</v>
+      </c>
+      <c r="X15" s="55" t="s">
+        <v>55</v>
       </c>
       <c r="Z15" s="55" t="s">
-        <v>88</v>
+        <v>333</v>
       </c>
       <c r="AA15" s="56" t="s">
-        <v>320</v>
+        <v>471</v>
       </c>
       <c r="AC15" t="s">
-        <v>321</v>
+        <v>466</v>
       </c>
       <c r="AD15" t="s">
-        <v>322</v>
+        <v>467</v>
       </c>
       <c r="AE15" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="AF15" s="11" t="s">
-        <v>55</v>
-      </c>
+        <v>476</v>
+      </c>
+      <c r="AF15" s="11"/>
       <c r="AG15" s="11" t="s">
-        <v>324</v>
+        <v>63</v>
       </c>
       <c r="AH15" s="11" t="s">
-        <v>326</v>
+        <v>469</v>
       </c>
       <c r="AI15" s="11" t="s">
-        <v>325</v>
+        <v>468</v>
       </c>
       <c r="AJ15" s="11" t="s">
-        <v>327</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="45">
@@ -5007,7 +5158,7 @@
         <v>245</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>328</v>
+        <v>478</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>53</v>
@@ -5018,7 +5169,9 @@
       <c r="L16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="M16" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="N16" s="14" t="s">
         <v>55</v>
       </c>
@@ -5037,23 +5190,20 @@
         <v>318</v>
       </c>
       <c r="W16" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="X16" s="14"/>
+        <v>484</v>
+      </c>
       <c r="Y16" s="14"/>
       <c r="Z16" s="14" t="s">
-        <v>333</v>
+        <v>479</v>
       </c>
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
       <c r="AC16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD16" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="AE16" s="14" t="s">
-        <v>329</v>
+        <v>482</v>
+      </c>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="15" t="s">
+        <v>485</v>
       </c>
       <c r="AF16" s="14" t="s">
         <v>55</v>
@@ -5062,11 +5212,13 @@
         <v>324</v>
       </c>
       <c r="AH16" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="AI16" s="15"/>
+        <v>480</v>
+      </c>
+      <c r="AI16" s="15" t="s">
+        <v>481</v>
+      </c>
       <c r="AJ16" s="15" t="s">
-        <v>331</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:36" ht="60">
@@ -8766,7 +8918,7 @@
     <row r="58" spans="1:36">
       <c r="H58" s="58">
         <f ca="1">TODAY()</f>
-        <v>42458</v>
+        <v>42470</v>
       </c>
     </row>
     <row r="59" spans="1:36">
@@ -8777,17 +8929,18 @@
     <row r="60" spans="1:36">
       <c r="H60">
         <f ca="1">H59-H58</f>
-        <v>2</v>
+        <v>-10</v>
       </c>
       <c r="I60" s="18">
         <f ca="1">H60*8</f>
-        <v>16</v>
+        <v>-80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1"/>
     <hyperlink ref="A6" r:id="rId2"/>
@@ -9004,16 +9157,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="28" customHeight="1">
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="Q1" s="64" t="s">
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="Q1" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
       <c r="AE1" s="38" t="s">
         <v>40</v>
       </c>

</xml_diff>